<commit_message>
Clarified the workflow for optimal IP assignment.
</commit_message>
<xml_diff>
--- a/Tutorial-04/Network IP Assignments.xlsx
+++ b/Tutorial-04/Network IP Assignments.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lectures\1701\lab1701\Tutorial-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818CED33-B484-4EAE-8958-42BAD7558948}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B4E151-4E3F-44EC-94FC-0BFA15D5AECC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="3270" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{018006E0-21FA-4D00-B9E3-B9488497F51C}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="17850" windowHeight="11910" xr2:uid="{018006E0-21FA-4D00-B9E3-B9488497F51C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="IP Ranges" sheetId="2" r:id="rId1"/>
     <sheet name="Network N1" sheetId="1" r:id="rId2"/>
     <sheet name="Network N2" sheetId="3" r:id="rId3"/>
     <sheet name="Network N5" sheetId="4" r:id="rId4"/>
@@ -305,6 +305,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -313,15 +322,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -639,7 +639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE589ACD-AECB-4282-90F6-276EB1AC036F}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -652,21 +652,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -678,7 +678,7 @@
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -690,7 +690,7 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -702,7 +702,7 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -714,7 +714,7 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -726,7 +726,7 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -738,7 +738,7 @@
       <c r="D7" s="2"/>
     </row>
     <row r="8" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -750,7 +750,7 @@
       <c r="D8" s="2"/>
     </row>
     <row r="9" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -762,7 +762,7 @@
       <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -774,7 +774,7 @@
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -807,12 +807,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -871,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36B1ADC-E415-4BAD-9C64-8E0B17949793}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -884,12 +884,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -961,12 +961,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="10"/>
     </row>
     <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">

</xml_diff>

<commit_message>
Improved .xlsx workbook for IP subnetting. Subnet masks of hosts are auto-completed from the IP ranges worksheet. New worksheet for static routes
</commit_message>
<xml_diff>
--- a/Tutorial-04/Network IP Assignments.xlsx
+++ b/Tutorial-04/Network IP Assignments.xlsx
@@ -8,15 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Lectures\1701\lab1701\Tutorial-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B4E151-4E3F-44EC-94FC-0BFA15D5AECC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080BF9D8-FC78-4846-8DD9-DFF6D8B484FB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="17850" windowHeight="11910" xr2:uid="{018006E0-21FA-4D00-B9E3-B9488497F51C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{018006E0-21FA-4D00-B9E3-B9488497F51C}"/>
   </bookViews>
   <sheets>
     <sheet name="IP Ranges" sheetId="2" r:id="rId1"/>
-    <sheet name="Network N1" sheetId="1" r:id="rId2"/>
-    <sheet name="Network N2" sheetId="3" r:id="rId3"/>
-    <sheet name="Network N5" sheetId="4" r:id="rId4"/>
+    <sheet name="Routers" sheetId="11" r:id="rId2"/>
+    <sheet name="Network N1" sheetId="1" r:id="rId3"/>
+    <sheet name="Network N2" sheetId="5" r:id="rId4"/>
+    <sheet name="Network N3" sheetId="6" r:id="rId5"/>
+    <sheet name="Network N4" sheetId="7" r:id="rId6"/>
+    <sheet name="Network N5" sheetId="8" r:id="rId7"/>
+    <sheet name="Network N6" sheetId="9" r:id="rId8"/>
+    <sheet name="Network N7" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,17 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="49">
   <si>
     <t>N1</t>
   </si>
   <si>
-    <t>Device</t>
-  </si>
-  <si>
-    <t>Network Interface</t>
-  </si>
-  <si>
     <t>IP Address</t>
   </si>
   <si>
@@ -57,12 +56,6 @@
     <t>Switch</t>
   </si>
   <si>
-    <t>Μέγεθος</t>
-  </si>
-  <si>
-    <t>Αναγνωριστικό CIDR</t>
-  </si>
-  <si>
     <t>Switch1-1</t>
   </si>
   <si>
@@ -142,13 +135,64 @@
   </si>
   <si>
     <t>Router 1 &lt;-&gt; 3</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>Hosts Count</t>
+  </si>
+  <si>
+    <t>Network Identifier (CIDR)</t>
+  </si>
+  <si>
+    <t>Subnet Mask (decimal-dotted)</t>
+  </si>
+  <si>
+    <t>Auto-completed from IP Ranges</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Network Interface Controller</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Next Hop IP Address</t>
+  </si>
+  <si>
+    <t>Static Routes</t>
+  </si>
+  <si>
+    <t>Remote Network Router Name</t>
+  </si>
+  <si>
+    <t>Router Name</t>
+  </si>
+  <si>
+    <t>Remote Network Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote Network Identifier (CIDR) </t>
+  </si>
+  <si>
+    <t>Remote Network Subnet Mask  (decimal-dotted)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +226,15 @@
       <name val="Arial Nova"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="161"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +253,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -287,23 +344,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -313,6 +373,33 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -637,10 +724,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE589ACD-AECB-4282-90F6-276EB1AC036F}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,227 +736,625 @@
     <col min="2" max="2" width="28.42578125" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
     <col min="4" max="4" width="43" customWidth="1"/>
+    <col min="5" max="5" width="44" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="7" t="s">
+      <c r="B6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:5" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+      <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="B11" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="C11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331FFA34-F3D1-4375-9B11-0BB1BEC277DA}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="5" max="5" width="28.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+    </row>
+    <row r="2" spans="1:7" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F38FF37-60E4-4893-8D3D-41B31EA32450}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:D7"/>
+      <selection activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A2</f>
+        <v>N1</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="7">
+        <f>'IP Ranges'!$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="7">
+        <f>'IP Ranges'!$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="7">
+        <f>'IP Ranges'!$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="7">
+        <f>'IP Ranges'!$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="7">
+        <f>'IP Ranges'!$E$2</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E36B1ADC-E415-4BAD-9C64-8E0B17949793}">
-  <dimension ref="A1:D7"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED9A0F47-6CC4-49C5-84A9-D9F925ADC370}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A3</f>
+        <v>N2</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="7">
+        <f>'IP Ranges'!$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="7">
+        <f>'IP Ranges'!$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="7">
+        <f>'IP Ranges'!$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="7">
+        <f>'IP Ranges'!$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="7">
+        <f>'IP Ranges'!$E$3</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC339270-5732-4FF2-A5C8-0D040EE9D0FF}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A4</f>
+        <v>N3</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="9">
+        <f>'IP Ranges'!E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="9">
+        <f>'IP Ranges'!E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="9">
+        <f>'IP Ranges'!E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="9">
+        <f>'IP Ranges'!E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="9">
+        <f>'IP Ranges'!E$4</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BE59B5E-D205-4DA2-B9C0-777ACAFA93E6}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -879,74 +1364,104 @@
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A5</f>
+        <v>N4</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="9">
+        <f>'IP Ranges'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="9">
+        <f>'IP Ranges'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="9">
+        <f>'IP Ranges'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="9">
+        <f>'IP Ranges'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="9">
+        <f>'IP Ranges'!E$5</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FD60A7-F86F-427A-8E5F-9025554EE7A1}">
-  <dimension ref="A1:D7"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DB9AF2-C3DE-4FBB-801F-F45E1F3F7793}">
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -956,65 +1471,309 @@
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="10"/>
-    </row>
-    <row r="2" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A6</f>
+        <v>N5</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="9">
+        <f>'IP Ranges'!E$6</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="9">
+        <f>'IP Ranges'!E$6</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="9">
+        <f>'IP Ranges'!E$6</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="9">
+        <f>'IP Ranges'!E$6</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="D7" s="9">
+        <f>'IP Ranges'!E$6</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AD50B65-B51B-4177-BFD0-BDBEA14E4B0B}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A7</f>
+        <v>N6</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="9">
+        <f>'IP Ranges'!E$7</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="9">
+        <f>'IP Ranges'!E$7</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="9">
+        <f>'IP Ranges'!E$7</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="9">
+        <f>'IP Ranges'!E$7</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="9">
+        <f>'IP Ranges'!E$7</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F7DC30E-D18A-445B-9548-87D7E4B521B8}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="25" customWidth="1"/>
+    <col min="3" max="4" width="28.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="str">
+        <f>'IP Ranges'!A8</f>
+        <v>N7</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="9">
+        <f>'IP Ranges'!E$8</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="9">
+        <f>'IP Ranges'!E$8</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="9">
+        <f>'IP Ranges'!E$8</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="9">
+        <f>'IP Ranges'!E$8</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="9">
+        <f>'IP Ranges'!E$8</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>